<commit_message>
Completed Implementation Constraints Plan
</commit_message>
<xml_diff>
--- a/Planning/Implementation Constraints Plan.xlsx
+++ b/Planning/Implementation Constraints Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/craig/codeclan_work/week_05/SportsLeagueApp/Planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/craig/codeclan_work/week_05/SportsLeagueWebApp/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C63C75F-D5DC-014D-BBCB-CA3B58EE692C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942C9B11-22DE-294C-B541-2320CC4C94FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16300" xr2:uid="{7F16F4AD-9309-8A42-BE43-27F0FE18B0CE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7F16F4AD-9309-8A42-BE43-27F0FE18B0CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Constraint Catergory</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>Just make sure when presenting the final solution that the local domain is running in the background</t>
+  </si>
+  <si>
+    <t>Must be fairly responsive when the user is interacting with the web application</t>
+  </si>
+  <si>
+    <t>Be efficient with the data being stored so it can be retrieved within a good response time.</t>
+  </si>
+  <si>
+    <t>Don't waste stoarge space needlessly.</t>
+  </si>
+  <si>
+    <t>Use only free software, web hosting and extenstions</t>
+  </si>
+  <si>
+    <t>Plan well, achieve the MVP and then re-plan time well to not run over.</t>
+  </si>
+  <si>
+    <t>Macbook being used for the project only has 512Gb internal storage</t>
+  </si>
+  <si>
+    <t>Must be usable by all people, possibly including people with colour-blindness</t>
+  </si>
+  <si>
+    <t>Use colour-blind friendly colour within project.</t>
   </si>
 </sst>
 </file>
@@ -463,7 +487,7 @@
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,44 +519,60 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" ht="68" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
       </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="2:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>

</xml_diff>